<commit_message>
Extract target rate and changes
Former-commit-id: 2c4a8f38047f69b962109d0bdb3f11a43d265b8c
</commit_message>
<xml_diff>
--- a/simplified_metadata_scraper/Matlab/Output/Bluebook/CSV/CommentedFiles/SentencesA_commented.xlsx
+++ b/simplified_metadata_scraper/Matlab/Output/Bluebook/CSV/CommentedFiles/SentencesA_commented.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10412"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivergiesecke/Dropbox/MPCounterfactual/simplified_metadata_scraper/Matlab/Output/Bluebook/CSV/CommentedFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B9D96935-3F71-F84B-B349-186BAFEB8027}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559A42AE-68C4-2E4C-8FAB-DD88315C9310}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28080" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28080" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SentencesA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -3289,7 +3289,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -3426,7 +3426,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3612,6 +3612,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3773,10 +3779,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4131,14 +4139,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V376"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="D348" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="J347" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G352" sqref="G352"/>
+      <selection pane="bottomRight" activeCell="Q353" sqref="Q353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14857,47 +14865,47 @@
         <v>1061</v>
       </c>
     </row>
-    <row r="367" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="A367">
+    <row r="367" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A367" s="3">
         <v>2008</v>
       </c>
-      <c r="B367" s="1">
+      <c r="B367" s="4">
         <v>39476</v>
       </c>
-      <c r="C367" s="1">
+      <c r="C367" s="4">
         <v>39477</v>
       </c>
-      <c r="D367">
+      <c r="D367" s="3">
         <v>5</v>
       </c>
-      <c r="E367">
+      <c r="E367" s="3">
         <v>3.5</v>
       </c>
-      <c r="F367">
+      <c r="F367" s="3">
         <v>3</v>
       </c>
-      <c r="G367" t="s">
+      <c r="G367" s="3" t="s">
         <v>986</v>
       </c>
-      <c r="H367" t="s">
+      <c r="H367" s="3" t="s">
         <v>987</v>
       </c>
-      <c r="I367" t="s">
+      <c r="I367" s="3" t="s">
         <v>988</v>
       </c>
-      <c r="J367" t="s">
+      <c r="J367" s="3" t="s">
         <v>989</v>
       </c>
-      <c r="Q367" s="2" t="s">
+      <c r="Q367" s="3" t="s">
         <v>1044</v>
       </c>
-      <c r="R367" s="2" t="s">
+      <c r="R367" s="3" t="s">
         <v>1059</v>
       </c>
-      <c r="S367" s="2">
+      <c r="S367" s="3">
         <v>-0.75</v>
       </c>
-      <c r="T367" s="2" t="s">
+      <c r="T367" s="3" t="s">
         <v>1057</v>
       </c>
     </row>

</xml_diff>